<commit_message>
Fixed tests after changes this morning.
</commit_message>
<xml_diff>
--- a/documentation/opcodes-completed.xlsx
+++ b/documentation/opcodes-completed.xlsx
@@ -1614,7 +1614,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.01171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2477,7 +2477,7 @@
       <c r="B17" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="4" t="s">
         <v>267</v>
       </c>
       <c r="D17" s="5" t="s">

</xml_diff>

<commit_message>
Added rest of return codes
</commit_message>
<xml_diff>
--- a/documentation/opcodes-completed.xlsx
+++ b/documentation/opcodes-completed.xlsx
@@ -1614,7 +1614,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.01171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2339,7 +2339,7 @@
       <c r="I14" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="J14" s="4" t="s">
         <v>224</v>
       </c>
       <c r="K14" s="5" t="s">
@@ -2392,7 +2392,7 @@
       <c r="I15" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="J15" s="4" t="s">
         <v>241</v>
       </c>
       <c r="K15" s="5" t="s">
@@ -2421,7 +2421,7 @@
       <c r="A16" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>250</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -2445,7 +2445,7 @@
       <c r="I16" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="J16" s="4" t="s">
         <v>258</v>
       </c>
       <c r="K16" s="5" t="s">
@@ -2474,7 +2474,7 @@
       <c r="A17" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>266</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -2498,7 +2498,7 @@
       <c r="I17" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J17" s="4" t="s">
         <v>274</v>
       </c>
       <c r="K17" s="7" t="s">

</xml_diff>

<commit_message>
Added half the JUMP instructions
</commit_message>
<xml_diff>
--- a/documentation/opcodes-completed.xlsx
+++ b/documentation/opcodes-completed.xlsx
@@ -1614,7 +1614,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
+      <selection pane="topLeft" activeCell="M24" activeCellId="0" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.01171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2321,7 +2321,7 @@
       <c r="C14" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>218</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -2374,7 +2374,7 @@
       <c r="C15" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>235</v>
       </c>
       <c r="E15" s="6" t="s">
@@ -2427,7 +2427,7 @@
       <c r="C16" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>252</v>
       </c>
       <c r="E16" s="7" t="s">
@@ -2480,7 +2480,7 @@
       <c r="C17" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>268</v>
       </c>
       <c r="E17" s="6" t="s">

</xml_diff>